<commit_message>
SauceDemo updated, 70% done
</commit_message>
<xml_diff>
--- a/src/test/java/loginDataSauce.xlsx
+++ b/src/test/java/loginDataSauce.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Djole\IdeaProjects\SauceDemoProject\src\test\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08DCCD70-DD22-49E9-9535-52A231D48C17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5581801-7600-47D9-A1C2-671B67747A90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20835" yWindow="750" windowWidth="16140" windowHeight="11595" xr2:uid="{ADB3B091-E726-49C6-9877-0B9BEA23FB76}"/>
+    <workbookView xWindow="20025" yWindow="855" windowWidth="16140" windowHeight="11595" xr2:uid="{ADB3B091-E726-49C6-9877-0B9BEA23FB76}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>firstname</t>
   </si>
@@ -42,13 +42,40 @@
     <t>Djordje</t>
   </si>
   <si>
-    <t>asdas</t>
-  </si>
-  <si>
-    <t>asdasd</t>
-  </si>
-  <si>
     <t>11090</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Doe</t>
+  </si>
+  <si>
+    <t>11323</t>
+  </si>
+  <si>
+    <t>Mikel</t>
+  </si>
+  <si>
+    <t>Andjelo</t>
+  </si>
+  <si>
+    <t>123123</t>
+  </si>
+  <si>
+    <t>Zorz</t>
+  </si>
+  <si>
+    <t>Sam</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>123122</t>
+  </si>
+  <si>
+    <t>223412</t>
   </si>
 </sst>
 </file>
@@ -404,7 +431,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -428,51 +455,51 @@
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>